<commit_message>
Week 15 a_b testing
</commit_message>
<xml_diff>
--- a/Week14/Day6/DailyChallenge/example_workbook.xlsx
+++ b/Week14/Day6/DailyChallenge/example_workbook.xlsx
@@ -435,27 +435,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>student</t>
+          <t>Student</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>math</t>
+          <t>Math</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>science</t>
+          <t>Science</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>english</t>
+          <t>English</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>gym</t>
+          <t>Gym</t>
         </is>
       </c>
     </row>

</xml_diff>